<commit_message>
list out all sheets
</commit_message>
<xml_diff>
--- a/resource/test.xlsx
+++ b/resource/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="510" windowWidth="13095" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="510" yWindow="510" windowWidth="13095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sample xsheet C" sheetId="1" r:id="rId1"/>
@@ -27,15 +27,6 @@
     <t>Salary</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>Dean</t>
-  </si>
-  <si>
     <t>Chris Wong A</t>
   </si>
   <si>
@@ -52,6 +43,15 @@
   </si>
   <si>
     <t>Chris Wong 1999</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Chris Wong</t>
+  </si>
+  <si>
+    <t>chriswong</t>
   </si>
 </sst>
 </file>
@@ -392,9 +392,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -412,7 +480,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>1500000</v>
@@ -423,7 +491,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>800000</v>
@@ -434,7 +502,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>700000</v>
@@ -537,7 +605,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>198200</v>
@@ -548,7 +616,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>201300</v>
@@ -559,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>199999</v>
@@ -574,7 +642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -662,7 +730,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>100000</v>
@@ -673,7 +741,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>200000</v>
@@ -684,7 +752,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>300000</v>

</xml_diff>